<commit_message>
Argparse & QML integration
</commit_message>
<xml_diff>
--- a/需求文档/多相流模拟软件multflow开发报价2023.xlsx
+++ b/需求文档/多相流模拟软件multflow开发报价2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\22846\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\home\repo\Multiflow\需求文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309B4080-65CC-4287-8211-1B768373F451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907702E9-821A-4437-8781-572993591F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6670" yWindow="4690" windowWidth="28800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -310,7 +310,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Microsoft YaHei"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>泡状流、段塞流、过渡流、搅动流、环雾流、分层流（水平管中出现）</t>
     </r>
@@ -319,7 +319,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <rFont val="Microsoft YaHei"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t>）、温度（每一相/总体）、压力、持液率、质量流量、体积流量、质量分数、体积分数、速度（每一相）、摩阻情况。</t>
     </r>
@@ -402,50 +402,47 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFC00000"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFC00000"/>
       <name val="Microsoft YaHei"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Microsoft YaHei"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -458,7 +455,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Microsoft YaHei"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -468,12 +465,18 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -540,18 +543,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -563,25 +566,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -590,21 +581,42 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -880,19 +892,19 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="7" style="3" customWidth="1"/>
     <col min="2" max="2" width="39.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.53125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="83.1328125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="35.86328125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="83.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="35.83203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="43" style="3" customWidth="1"/>
-    <col min="7" max="7" width="20.86328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.53125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="3" customWidth="1"/>
     <col min="9" max="9" width="15" style="3" customWidth="1"/>
     <col min="10" max="16384" width="9" style="3"/>
   </cols>
@@ -951,431 +963,431 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="13" customFormat="1" ht="61.15" customHeight="1">
-      <c r="A3" s="12">
+    <row r="3" spans="1:9" s="15" customFormat="1" ht="61.15" customHeight="1">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>59</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="I3" s="12"/>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="109.25" customHeight="1">
-      <c r="A4" s="15">
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" s="18" customFormat="1" ht="109.25" customHeight="1">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" ht="97.25" customHeight="1">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="10" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="8"/>
+      <c r="G5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="10"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A6" s="15">
+      <c r="A6" s="11">
         <v>4</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15" t="s">
+      <c r="G6" s="11"/>
+      <c r="H6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" ht="70.25" customHeight="1">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" ht="39" customHeight="1">
-      <c r="A8" s="15">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" s="18" customFormat="1" ht="39" customHeight="1">
+      <c r="A8" s="19">
         <v>5</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" ht="40.799999999999997" customHeight="1">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="10" t="s">
+    <row r="9" spans="1:9" s="18" customFormat="1" ht="40.75" customHeight="1">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="10" t="s">
+      <c r="G9" s="19"/>
+      <c r="H9" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="15"/>
+      <c r="I9" s="19"/>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1" ht="17" customHeight="1">
-      <c r="A10" s="15">
+      <c r="A10" s="11">
         <v>6</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="15"/>
+      <c r="I10" s="11"/>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1" ht="17" customHeight="1">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1" ht="85.25" customHeight="1">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1" ht="106.25" customHeight="1">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-    </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" ht="105.6" customHeight="1">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="11" t="s">
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" ht="105.65" customHeight="1">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-    </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" ht="91.8" customHeight="1">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15" t="s">
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" s="1" customFormat="1" ht="91.75" customHeight="1">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1" ht="84" customHeight="1">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="11" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-    </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" ht="90.6" customHeight="1">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="11" t="s">
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" spans="1:9" s="1" customFormat="1" ht="90.65" customHeight="1">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-    </row>
-    <row r="18" spans="1:9" s="1" customFormat="1" ht="105.6" customHeight="1">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="11" t="s">
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" spans="1:9" s="1" customFormat="1" ht="105.65" customHeight="1">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-    </row>
-    <row r="19" spans="1:9" s="1" customFormat="1" ht="31.05" customHeight="1">
-      <c r="A19" s="10">
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="1:9" s="1" customFormat="1" ht="31" customHeight="1">
+      <c r="A19" s="8">
         <v>7</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10" t="s">
+      <c r="G19" s="8"/>
+      <c r="H19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="10"/>
-    </row>
-    <row r="20" spans="1:9" s="1" customFormat="1" ht="22.25" customHeight="1">
-      <c r="A20" s="18">
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="1:9" s="18" customFormat="1" ht="22.25" customHeight="1">
+      <c r="A20" s="20">
         <v>8</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15" t="s">
+      <c r="E20" s="19"/>
+      <c r="F20" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G20" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H20" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I20" s="15"/>
-    </row>
-    <row r="21" spans="1:9" s="1" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A21" s="19"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-    </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A22" s="20"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-    </row>
-    <row r="23" spans="1:9" s="1" customFormat="1" ht="45.4" customHeight="1">
-      <c r="A23" s="10">
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" s="18" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A21" s="22"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+    </row>
+    <row r="22" spans="1:9" s="18" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A22" s="23"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+    </row>
+    <row r="23" spans="1:9" s="18" customFormat="1" ht="45.4" customHeight="1">
+      <c r="A23" s="16">
         <v>9</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10" t="s">
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="10"/>
-    </row>
-    <row r="24" spans="1:9" s="1" customFormat="1" ht="82.05" customHeight="1">
-      <c r="A24" s="10">
+      <c r="I23" s="16"/>
+    </row>
+    <row r="24" spans="1:9" s="1" customFormat="1" ht="82" customHeight="1">
+      <c r="A24" s="8">
         <v>10</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10" t="s">
+      <c r="E24" s="8"/>
+      <c r="F24" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="G24" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I24" s="10"/>
+      <c r="I24" s="8"/>
     </row>
     <row r="25" spans="1:9" s="2" customFormat="1" ht="22.5" customHeight="1">
       <c r="A25" s="6">
@@ -1392,7 +1404,7 @@
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="15"/>
+      <c r="G25" s="11"/>
       <c r="H25" s="6" t="s">
         <v>39</v>
       </c>
@@ -1400,106 +1412,84 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A26" s="10">
+    <row r="26" spans="1:9" s="18" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A26" s="16">
         <v>12</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="10" t="s">
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I26" s="10"/>
-    </row>
-    <row r="27" spans="1:9" s="1" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A27" s="10">
+      <c r="I26" s="16"/>
+    </row>
+    <row r="27" spans="1:9" s="18" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A27" s="16">
         <v>13</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10" t="s">
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I27" s="10"/>
-    </row>
-    <row r="28" spans="1:9" s="1" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A28" s="10">
+      <c r="I27" s="16"/>
+    </row>
+    <row r="28" spans="1:9" s="18" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A28" s="16">
         <v>14</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="9" t="s">
+      <c r="C28" s="16"/>
+      <c r="D28" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10" t="s">
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="10"/>
+      <c r="I28" s="16"/>
     </row>
     <row r="29" spans="1:9" s="1" customFormat="1" ht="22.5" customHeight="1">
-      <c r="A29" s="10">
+      <c r="A29" s="8">
         <v>15</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H10:H18"/>
-    <mergeCell ref="H20:H22"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I10:I18"/>
-    <mergeCell ref="I20:I22"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="F15:F18"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G18"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="A6:A7"/>
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A8:A9"/>
@@ -1515,6 +1505,28 @@
     <mergeCell ref="C15:C18"/>
     <mergeCell ref="C20:C22"/>
     <mergeCell ref="D6:D7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I18"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="F15:F18"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G18"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H10:H18"/>
+    <mergeCell ref="H20:H22"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="A6:A7"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>